<commit_message>
Updated burnup chart, added sprint 3 report, updated typo in sprint 2 report
</commit_message>
<xml_diff>
--- a/Burnup_Chart.xlsx
+++ b/Burnup_Chart.xlsx
@@ -166,9 +166,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Done</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -254,18 +251,33 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -275,9 +287,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Total</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -363,10 +372,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>116</c:v>
                 </c:pt>
@@ -375,6 +384,21 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -392,11 +416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="343696592"/>
-        <c:axId val="343702472"/>
+        <c:axId val="226318360"/>
+        <c:axId val="226323848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343696592"/>
+        <c:axId val="226318360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343702472"/>
+        <c:crossAx val="226323848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -502,7 +526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343702472"/>
+        <c:axId val="226323848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343696592"/>
+        <c:crossAx val="226318360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1536,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1603,7 @@
         <v>116</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,7 +1614,62 @@
         <v>142</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>161</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>161</v>
+      </c>
+      <c r="C6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>125</v>
+      </c>
+      <c r="C7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>125</v>
+      </c>
+      <c r="C8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+      <c r="C9">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>